<commit_message>
comment from python script
</commit_message>
<xml_diff>
--- a/actitud.xlsx
+++ b/actitud.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pablo\OneDrive\Github\1AB\1AB\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ef4cc4ddfd4d7cd1/Github/1AB/1AB/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FCA0849-8D95-4177-8758-69C1CE4C95AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="8" documentId="13_ncr:1_{0FCA0849-8D95-4177-8758-69C1CE4C95AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{020E3F45-7668-48CD-8098-A990DB6507DD}"/>
   <bookViews>
-    <workbookView xWindow="15360" yWindow="0" windowWidth="15360" windowHeight="16680" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Astronauta" sheetId="1" r:id="rId1"/>
@@ -497,8 +497,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1207,8 +1207,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D45A07B9-F651-41BC-A481-395AA628394B}">
   <dimension ref="A1:P21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1270,33 +1270,45 @@
       <c r="A2" t="s">
         <v>12</v>
       </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
       <c r="P2">
         <f>IFERROR(SUM(B2:O2)/COUNT(B2:O2)*100, 0)</f>
-        <v>0</v>
+        <v>100</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>13</v>
       </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
       <c r="P3">
         <f t="shared" ref="P3:P21" si="0">IFERROR(SUM(B3:O3)/COUNT(B3:O3)*100, 0)</f>
-        <v>0</v>
+        <v>100</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>14</v>
       </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
       <c r="P4">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>100</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>15</v>
       </c>
+      <c r="B5">
+        <v>0</v>
+      </c>
       <c r="P5">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1306,51 +1318,69 @@
       <c r="A6" t="s">
         <v>16</v>
       </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
       <c r="P6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>100</v>
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>17</v>
       </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
       <c r="P7">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>100</v>
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>18</v>
       </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
       <c r="P8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>100</v>
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>19</v>
       </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
       <c r="P9">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>100</v>
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>20</v>
       </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
       <c r="P10">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>100</v>
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>21</v>
       </c>
+      <c r="B11">
+        <v>0</v>
+      </c>
       <c r="P11">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1360,90 +1390,120 @@
       <c r="A12" t="s">
         <v>22</v>
       </c>
+      <c r="B12">
+        <v>1</v>
+      </c>
       <c r="P12">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>100</v>
       </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>23</v>
       </c>
+      <c r="B13">
+        <v>1</v>
+      </c>
       <c r="P13">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>100</v>
       </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>24</v>
       </c>
+      <c r="B14">
+        <v>1</v>
+      </c>
       <c r="P14">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>100</v>
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>25</v>
       </c>
+      <c r="B15">
+        <v>1</v>
+      </c>
       <c r="P15">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>100</v>
       </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>26</v>
       </c>
+      <c r="B16">
+        <v>1</v>
+      </c>
       <c r="P16">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>100</v>
       </c>
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>27</v>
       </c>
+      <c r="B17">
+        <v>1</v>
+      </c>
       <c r="P17">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>100</v>
       </c>
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>28</v>
       </c>
+      <c r="B18">
+        <v>1</v>
+      </c>
       <c r="P18">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>100</v>
       </c>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>29</v>
       </c>
+      <c r="B19">
+        <v>1</v>
+      </c>
       <c r="P19">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>100</v>
       </c>
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>30</v>
       </c>
+      <c r="B20">
+        <v>1</v>
+      </c>
       <c r="P20">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>100</v>
       </c>
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>31</v>
       </c>
+      <c r="B21">
+        <v>1</v>
+      </c>
       <c r="P21">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>100</v>
       </c>
     </row>
   </sheetData>

</xml_diff>